<commit_message>
Updating Capstone Documents, Archiving Old Reports
</commit_message>
<xml_diff>
--- a/Project Documentation/Capstone Documents/Hagerman_Kendrick_Risk_Matricies.xlsx
+++ b/Project Documentation/Capstone Documents/Hagerman_Kendrick_Risk_Matricies.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kendrick\Documents\UWF Stuff\Capstone!\Week 5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kendrick\Documents\UWF Stuff\Capstone!\Git Repo\FoodGiantFlyer\Project Documentation\Capstone Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Extensive</t>
   </si>
@@ -60,9 +60,6 @@
   </si>
   <si>
     <t>#102</t>
-  </si>
-  <si>
-    <t>#101</t>
   </si>
   <si>
     <t>#201</t>
@@ -473,34 +470,32 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="8.44140625" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
-      <c r="F1" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="F1" s="4"/>
       <c r="G1" s="4"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -512,20 +507,20 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -535,7 +530,7 @@
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
       <c r="D6" s="2" t="s">
         <v>11</v>
@@ -548,7 +543,7 @@
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -562,7 +557,7 @@
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="2"/>
@@ -573,7 +568,7 @@
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
     </row>
-    <row r="9" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>4</v>
       </c>
@@ -587,7 +582,7 @@
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
     </row>
-    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="C10" s="5" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Updating documentation post Progress Report 2. Removed unused user guide
</commit_message>
<xml_diff>
--- a/Project Documentation/Capstone Documents/Hagerman_Kendrick_Risk_Matricies.xlsx
+++ b/Project Documentation/Capstone Documents/Hagerman_Kendrick_Risk_Matricies.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Extensive</t>
   </si>
@@ -57,12 +57,6 @@
   </si>
   <si>
     <t>#103</t>
-  </si>
-  <si>
-    <t>#102</t>
-  </si>
-  <si>
-    <t>#201</t>
   </si>
 </sst>
 </file>
@@ -470,7 +464,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,9 +513,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="4"/>
@@ -532,9 +524,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
-      <c r="D6" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="4"/>

</xml_diff>